<commit_message>
Finally figure out how to handle parameterized exchanges
</commit_message>
<xml_diff>
--- a/tests/fixtures/excel/export-complicated.xlsx
+++ b/tests/fixtures/excel/export-complicated.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28028"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="20740" windowHeight="16800"/>
   </bookViews>
   <sheets>
     <sheet name="example" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="39">
   <si>
     <t>Project parameters</t>
   </si>
@@ -128,13 +133,16 @@
   </si>
   <si>
     <t>sqrt(red - 20)</t>
+  </si>
+  <si>
+    <t>foo * bar + 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -467,14 +475,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -509,7 +526,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="15">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -525,7 +542,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" ht="15">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -569,7 +586,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" ht="15">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -593,7 +610,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -601,7 +618,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -609,12 +626,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:6" ht="15">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -631,7 +648,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -648,12 +665,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:6" ht="15">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -669,8 +686,11 @@
       <c r="E24" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -687,7 +707,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -700,8 +720,11 @@
       <c r="E26" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15">
       <c r="A28" s="1" t="s">
         <v>16</v>
       </c>
@@ -709,7 +732,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -717,7 +740,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -725,7 +748,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -733,7 +756,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:6" ht="15">
       <c r="A32" s="1" t="s">
         <v>25</v>
       </c>
@@ -772,7 +795,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" ht="15">
       <c r="A36" s="1" t="s">
         <v>27</v>
       </c>
@@ -807,5 +830,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Write and read AP group names, and reorganize code to allow writing sections separately
</commit_message>
<xml_diff>
--- a/tests/fixtures/excel/export-complicated.xlsx
+++ b/tests/fixtures/excel/export-complicated.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="40">
   <si>
     <t>Project parameters</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>foo * bar + 4</t>
+  </si>
+  <si>
+    <t>my group</t>
   </si>
 </sst>
 </file>
@@ -479,7 +482,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -630,6 +633,9 @@
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
@@ -759,6 +765,9 @@
     <row r="32" spans="1:6" ht="15">
       <c r="A32" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="B32" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:5">

</xml_diff>

<commit_message>
Fix changes in saving original amount of parameters
</commit_message>
<xml_diff>
--- a/tests/fixtures/excel/export-complicated.xlsx
+++ b/tests/fixtures/excel/export-complicated.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10210"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmutel/Code/bw2gh/io/tests/fixtures/excel/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179E5CC9-4F31-DD42-B135-30C8B6DEDE51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="20740" windowHeight="16800"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="20740" windowHeight="16800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="example" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="41">
   <si>
     <t>Project parameters</t>
   </si>
@@ -139,12 +145,15 @@
   </si>
   <si>
     <t>my group</t>
+  </si>
+  <si>
+    <t>original_amount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -191,6 +200,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -478,14 +495,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
@@ -494,12 +511,12 @@
     <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -510,7 +527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -521,7 +538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -529,7 +546,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15">
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -537,7 +554,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -545,12 +562,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15">
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -564,7 +581,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -575,7 +592,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -589,7 +606,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15">
+    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -597,7 +614,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -605,7 +622,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -613,7 +630,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -621,7 +638,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -629,7 +646,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15">
+    <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -637,7 +654,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -654,7 +671,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -671,12 +688,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15">
+    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -695,8 +712,11 @@
       <c r="F24" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -713,7 +733,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -729,8 +749,11 @@
       <c r="F26" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="15">
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>16</v>
       </c>
@@ -738,7 +761,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -746,7 +769,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -754,7 +777,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -762,7 +785,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15">
+    <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>25</v>
       </c>
@@ -770,7 +793,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -787,7 +810,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -804,12 +827,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15">
+    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -823,7 +846,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Fixes for bw2data 2.5 dev release
</commit_message>
<xml_diff>
--- a/tests/fixtures/excel/export-complicated.xlsx
+++ b/tests/fixtures/excel/export-complicated.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmutel/Code/bw2gh/io/tests/fixtures/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmutel/Code/bw2/io/tests/fixtures/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179E5CC9-4F31-DD42-B135-30C8B6DEDE51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24FEC42-411D-C141-863B-1697E6118655}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="20740" windowHeight="16800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="42">
   <si>
     <t>Project parameters</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>original_amount</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -496,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -632,231 +635,247 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" t="s">
-        <v>22</v>
+        <v>41</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>5</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>26</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>19</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" t="s">
-        <v>28</v>
-      </c>
-      <c r="F24" t="s">
-        <v>3</v>
-      </c>
-      <c r="G24" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25">
         <v>1</v>
       </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E25" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="F25" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>30</v>
       </c>
-      <c r="B26">
+      <c r="B27">
         <v>9</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>31</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E27" t="s">
         <v>32</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F27" t="s">
         <v>38</v>
       </c>
-      <c r="G26">
+      <c r="G27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+    <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>25</v>
+        <v>41</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>21</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>1</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B35" t="s">
         <v>2</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C35" t="s">
         <v>3</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D35" t="s">
         <v>18</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E35" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>36</v>
       </c>
-      <c r="B34">
+      <c r="B36">
         <v>3</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C36" t="s">
         <v>37</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D36" t="s">
         <v>33</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E36" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+    <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>1</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B39" t="s">
         <v>2</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C39" t="s">
         <v>21</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D39" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>30</v>
       </c>
-      <c r="B38">
+      <c r="B40">
         <v>10</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C40" t="s">
         <v>31</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D40" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Don't export id field in CSV/Export
</commit_message>
<xml_diff>
--- a/tests/fixtures/excel/export-complicated.xlsx
+++ b/tests/fixtures/excel/export-complicated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmutel/Code/bw2/io/tests/fixtures/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24FEC42-411D-C141-863B-1697E6118655}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3A161E-0531-6E44-AB80-577CCA2B9C8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="20740" windowHeight="16800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="41">
   <si>
     <t>Project parameters</t>
   </si>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>original_amount</t>
-  </si>
-  <si>
-    <t>id</t>
   </si>
 </sst>
 </file>
@@ -499,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -635,247 +632,231 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>1</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B24" t="s">
         <v>2</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" t="s">
         <v>3</v>
       </c>
-      <c r="D21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22">
-        <v>5</v>
-      </c>
-      <c r="C22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>27</v>
+      <c r="G24" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25">
         <v>1</v>
       </c>
-      <c r="B25" t="s">
-        <v>2</v>
-      </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E25" t="s">
-        <v>28</v>
-      </c>
-      <c r="F25" t="s">
-        <v>3</v>
-      </c>
-      <c r="G25" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B27">
-        <v>9</v>
-      </c>
-      <c r="C27" t="s">
-        <v>31</v>
-      </c>
-      <c r="E27" t="s">
-        <v>32</v>
-      </c>
-      <c r="F27" t="s">
-        <v>38</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>30</v>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>21</v>
+        <v>34</v>
+      </c>
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B34" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>1</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B37" t="s">
         <v>2</v>
       </c>
-      <c r="C35" t="s">
-        <v>3</v>
-      </c>
-      <c r="D35" t="s">
-        <v>18</v>
-      </c>
-      <c r="E35" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36">
-        <v>3</v>
-      </c>
-      <c r="C36" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" t="s">
-        <v>33</v>
-      </c>
-      <c r="E36" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="C37" t="s">
         <v>21</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D37" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>30</v>
       </c>
-      <c r="B40">
+      <c r="B38">
         <v>10</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C38" t="s">
         <v>31</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D38" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>